<commit_message>
changed scatter  and updated in xlsx file
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s542423\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s542423\Documents\GitHub\map-reduce-food_preference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{709019CF-90C6-4E9A-BE29-E82BF23EEAE3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DBB642-F33F-4E67-995F-8DAAD3D9D7C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{C53925D5-3DC7-4DB0-83C9-3AB587086DAA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C53925D5-3DC7-4DB0-83C9-3AB587086DAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -105,13 +105,27 @@
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
               <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  </a:sysClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -119,35 +133,44 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" b="1" i="0">
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Age</a:t>
+              <a:t>Age Food Preference</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" b="1" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" b="1" i="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Food</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" b="1" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" b="1" i="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Preference</a:t>
-            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -163,13 +186,27 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
-                </a:schemeClr>
+                </a:sysClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -202,7 +239,9 @@
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -224,288 +263,288 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$50</c:f>
+              <c:f>Sheet1!$A$2:$A$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="49"/>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>22</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>27</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>28</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>29</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>31</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>33</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="30">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="31">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
                   <c:v>44</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="33">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="34">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="35">
                   <c:v>47</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="36">
                   <c:v>49</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="37">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="38">
                   <c:v>51</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="39">
                   <c:v>53</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="40">
                   <c:v>54</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="41">
                   <c:v>56</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="42">
                   <c:v>59</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="43">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="44">
                   <c:v>63</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="45">
                   <c:v>65</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="46">
                   <c:v>67</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="47">
                   <c:v>74</c:v>
                 </c:pt>
-                <c:pt idx="46">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$50</c:f>
+              <c:f>Sheet1!$B$2:$B$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="49"/>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="30">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="31">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="37">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>2</c:v>
@@ -514,7 +553,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>1</c:v>
@@ -526,10 +565,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="47">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="48">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -537,7 +576,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-25EB-47CC-8FBE-CD7373E7F198}"/>
+              <c16:uniqueId val="{00000000-945F-4074-A087-93022BFD002B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -549,11 +588,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1459734544"/>
-        <c:axId val="1462296096"/>
+        <c:axId val="1160135327"/>
+        <c:axId val="1160133247"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1459734544"/>
+        <c:axId val="1160135327"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -610,12 +649,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1462296096"/>
+        <c:crossAx val="1160133247"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1462296096"/>
+        <c:axId val="1160133247"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -672,7 +711,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1459734544"/>
+        <c:crossAx val="1160135327"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1282,22 +1321,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>119061</xdr:rowOff>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:colOff>220980</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:rowOff>179070</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52F0E5C3-1166-4D89-8734-A282C9008079}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{796EC7EF-8AEB-4D2D-B67F-633C7349D7BE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1618,15 +1657,15 @@
   <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1634,399 +1673,402 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>18</v>
       </c>
-      <c r="B7">
+      <c r="B9">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
         <v>19</v>
       </c>
-      <c r="B8">
+      <c r="B10">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
         <v>20</v>
       </c>
-      <c r="B9">
+      <c r="B11">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>21</v>
       </c>
-      <c r="B10">
+      <c r="B12">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>22</v>
       </c>
-      <c r="B11">
+      <c r="B13">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
         <v>23</v>
       </c>
-      <c r="B12">
+      <c r="B14">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>24</v>
       </c>
-      <c r="B13">
+      <c r="B15">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>25</v>
       </c>
-      <c r="B14">
+      <c r="B16">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
         <v>26</v>
       </c>
-      <c r="B15">
+      <c r="B17">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>27</v>
       </c>
-      <c r="B16">
+      <c r="B18">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>28</v>
       </c>
-      <c r="B17">
+      <c r="B19">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
         <v>29</v>
       </c>
-      <c r="B18">
+      <c r="B20">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
         <v>30</v>
       </c>
-      <c r="B19">
+      <c r="B21">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
         <v>31</v>
       </c>
-      <c r="B20">
+      <c r="B22">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
         <v>32</v>
       </c>
-      <c r="B21">
+      <c r="B23">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
         <v>33</v>
       </c>
-      <c r="B22">
+      <c r="B24">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
         <v>34</v>
       </c>
-      <c r="B23">
+      <c r="B25">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
         <v>35</v>
       </c>
-      <c r="B24">
+      <c r="B26">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
         <v>36</v>
       </c>
-      <c r="B25">
+      <c r="B27">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
         <v>37</v>
       </c>
-      <c r="B26">
+      <c r="B28">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29">
         <v>38</v>
       </c>
-      <c r="B27">
+      <c r="B29">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30">
         <v>39</v>
       </c>
-      <c r="B28">
+      <c r="B30">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31">
         <v>40</v>
       </c>
-      <c r="B29">
+      <c r="B31">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32">
         <v>42</v>
       </c>
-      <c r="B30">
+      <c r="B32">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
         <v>43</v>
       </c>
-      <c r="B31">
+      <c r="B33">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
         <v>44</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>45</v>
-      </c>
-      <c r="B33">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>46</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B37">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
+        <v>50</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>51</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41">
         <v>53</v>
       </c>
-      <c r="B39">
+      <c r="B41">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42">
         <v>54</v>
       </c>
-      <c r="B40">
+      <c r="B42">
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43">
         <v>56</v>
-      </c>
-      <c r="B41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>59</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>60</v>
       </c>
       <c r="B43">
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B44">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B46">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B47">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
+        <v>74</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50">
         <v>80</v>
       </c>
-      <c r="B49">
+      <c r="B50">
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>9</v>
-      </c>
-      <c r="B50">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B50">
+    <sortCondition ref="A2:A50"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>